<commit_message>
Update version to V5.1
</commit_message>
<xml_diff>
--- a/templates tasmota.xlsx
+++ b/templates tasmota.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/talesmaschio/Library/CloudStorage/Dropbox/GitHub/Kicad/ESP-24v-16ch/V2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tales.maschio\Documents\Git\esp-24v-16ch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DFA660-332A-7843-B946-90A3DCF35679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B800297E-86F8-4BEF-9A2E-8A4DCD99EFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="960" windowWidth="30520" windowHeight="19360" xr2:uid="{EEB84482-71D0-4740-9A7C-C6470B96A6C1}"/>
+    <workbookView xWindow="25950" yWindow="585" windowWidth="23895" windowHeight="19995" xr2:uid="{EEB84482-71D0-4740-9A7C-C6470B96A6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -148,13 +148,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,7 +213,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -319,7 +319,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,7 +461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -472,17 +472,17 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -490,364 +490,364 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>3200</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>3232</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>5536</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <v>5536</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>10240</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
         <v>10241</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1">
         <v>5600</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="1">
         <v>5600</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3">
-        <v>0</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1">
         <v>5568</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="1">
         <v>5568</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3">
-        <v>0</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3">
-        <v>0</v>
-      </c>
-      <c r="C28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3">
-        <v>0</v>
-      </c>
-      <c r="C29" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3">
-        <v>0</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
         <v>608</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
         <v>640</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3">
-        <v>1</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>